<commit_message>
Ahora se carga el contenido de la matríz en el arreglo bidimensional de manera correcta
</commit_message>
<xml_diff>
--- a/src/main/resources/matrix.xlsx
+++ b/src/main/resources/matrix.xlsx
@@ -76,7 +76,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -85,6 +85,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -333,22 +336,22 @@
       <c r="A2" s="3">
         <v>0.0</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="4">
         <v>1.0</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="4">
         <v>39.0</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="4">
         <v>500.0</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="4">
         <v>0.0</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="4">
         <v>0.0</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="4">
         <v>0.0</v>
       </c>
     </row>
@@ -356,22 +359,22 @@
       <c r="A3" s="3">
         <v>1.0</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="4">
         <v>2.0</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="4">
         <v>3.0</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="4">
         <v>-1.0</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="4">
         <v>-1.0</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="4">
         <v>-1.0</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="4">
         <v>-1.0</v>
       </c>
     </row>
@@ -379,22 +382,22 @@
       <c r="A4" s="3">
         <v>2.0</v>
       </c>
-      <c r="B4" s="3">
-        <v>-2.0</v>
-      </c>
-      <c r="C4" s="3">
-        <v>-2.0</v>
-      </c>
-      <c r="D4" s="3">
-        <v>-2.0</v>
-      </c>
-      <c r="E4" s="3">
-        <v>-2.0</v>
-      </c>
-      <c r="F4" s="3">
-        <v>-2.0</v>
-      </c>
-      <c r="G4" s="3">
+      <c r="B4" s="4">
+        <v>-2.0</v>
+      </c>
+      <c r="C4" s="4">
+        <v>-2.0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>-2.0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>-2.0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>-2.0</v>
+      </c>
+      <c r="G4" s="4">
         <v>-2.0</v>
       </c>
     </row>
@@ -402,22 +405,22 @@
       <c r="A5" s="3">
         <v>3.0</v>
       </c>
-      <c r="B5" s="3">
-        <v>-3.0</v>
-      </c>
-      <c r="C5" s="3">
-        <v>-3.0</v>
-      </c>
-      <c r="D5" s="3">
-        <v>-3.0</v>
-      </c>
-      <c r="E5" s="3">
-        <v>-3.0</v>
-      </c>
-      <c r="F5" s="3">
-        <v>-3.0</v>
-      </c>
-      <c r="G5" s="3">
+      <c r="B5" s="4">
+        <v>-3.0</v>
+      </c>
+      <c r="C5" s="4">
+        <v>-3.0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>-3.0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>-3.0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>-3.0</v>
+      </c>
+      <c r="G5" s="4">
         <v>-3.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se juntó la columna de letras minúsculas y mayúsculas
</commit_message>
<xml_diff>
--- a/src/main/resources/matrix.xlsx
+++ b/src/main/resources/matrix.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>+</t>
   </si>
@@ -96,10 +96,7 @@
     <t>0-9</t>
   </si>
   <si>
-    <t>a-z</t>
-  </si>
-  <si>
-    <t>A-Z</t>
+    <t>a-Z</t>
   </si>
   <si>
     <t>@</t>
@@ -768,7 +765,7 @@
   <sheetFormatPr defaultColWidth="12.630000000000001" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col customWidth="1" min="1" max="1" style="1" width="5.7109375"/>
-    <col customWidth="1" min="2" max="36" width="5.7109375"/>
+    <col customWidth="1" min="2" max="35" width="5.7109375"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -863,7 +860,7 @@
       <c r="AE1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AF1" s="2" t="s">
         <v>30</v>
       </c>
       <c r="AG1" s="2" t="s">
@@ -874,9 +871,6 @@
       </c>
       <c r="AI1" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="AJ1" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2">
@@ -970,11 +964,11 @@
       <c r="AD2" s="4">
         <v>64</v>
       </c>
-      <c r="AE2" s="4">
-        <v>64</v>
-      </c>
-      <c r="AF2" s="5">
+      <c r="AE2" s="5">
         <v>500</v>
+      </c>
+      <c r="AF2" s="4">
+        <v>0</v>
       </c>
       <c r="AG2" s="4">
         <v>0</v>
@@ -982,10 +976,7 @@
       <c r="AH2" s="4">
         <v>0</v>
       </c>
-      <c r="AI2" s="4">
-        <v>0</v>
-      </c>
-      <c r="AJ2" s="5">
+      <c r="AI2" s="5">
         <v>500</v>
       </c>
     </row>
@@ -1095,9 +1086,6 @@
       <c r="AI3" s="6">
         <v>-1</v>
       </c>
-      <c r="AJ3" s="6">
-        <v>-1</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="2">
@@ -1205,9 +1193,6 @@
       <c r="AI4" s="6">
         <v>-2</v>
       </c>
-      <c r="AJ4" s="6">
-        <v>-2</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="2">
@@ -1315,9 +1300,6 @@
       <c r="AI5" s="6">
         <v>-3</v>
       </c>
-      <c r="AJ5" s="6">
-        <v>-3</v>
-      </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="7">
@@ -1425,9 +1407,6 @@
       <c r="AI6" s="6">
         <v>-4</v>
       </c>
-      <c r="AJ6" s="6">
-        <v>-4</v>
-      </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="2">
@@ -1535,9 +1514,6 @@
       <c r="AI7" s="6">
         <v>-5</v>
       </c>
-      <c r="AJ7" s="6">
-        <v>-5</v>
-      </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="2">
@@ -1645,9 +1621,6 @@
       <c r="AI8" s="6">
         <v>-6</v>
       </c>
-      <c r="AJ8" s="6">
-        <v>-6</v>
-      </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="2">
@@ -1755,9 +1728,6 @@
       <c r="AI9" s="6">
         <v>-7</v>
       </c>
-      <c r="AJ9" s="6">
-        <v>-7</v>
-      </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="2">
@@ -1865,9 +1835,6 @@
       <c r="AI10" s="6">
         <v>-8</v>
       </c>
-      <c r="AJ10" s="6">
-        <v>-8</v>
-      </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="7">
@@ -1975,9 +1942,6 @@
       <c r="AI11" s="6">
         <v>-9</v>
       </c>
-      <c r="AJ11" s="6">
-        <v>-9</v>
-      </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="2">
@@ -2085,9 +2049,6 @@
       <c r="AI12" s="6">
         <v>-10</v>
       </c>
-      <c r="AJ12" s="6">
-        <v>-10</v>
-      </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="2">
@@ -2195,9 +2156,6 @@
       <c r="AI13" s="6">
         <v>-11</v>
       </c>
-      <c r="AJ13" s="6">
-        <v>-11</v>
-      </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="2">
@@ -2305,9 +2263,6 @@
       <c r="AI14" s="6">
         <v>-12</v>
       </c>
-      <c r="AJ14" s="6">
-        <v>-12</v>
-      </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="2">
@@ -2415,9 +2370,6 @@
       <c r="AI15" s="6">
         <v>-13</v>
       </c>
-      <c r="AJ15" s="6">
-        <v>-13</v>
-      </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="7">
@@ -2525,9 +2477,6 @@
       <c r="AI16" s="6">
         <v>-14</v>
       </c>
-      <c r="AJ16" s="6">
-        <v>-14</v>
-      </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="2">
@@ -2635,9 +2584,6 @@
       <c r="AI17" s="6">
         <v>-15</v>
       </c>
-      <c r="AJ17" s="6">
-        <v>-15</v>
-      </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="2">
@@ -2745,9 +2691,6 @@
       <c r="AI18" s="6">
         <v>-16</v>
       </c>
-      <c r="AJ18" s="6">
-        <v>-16</v>
-      </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="2">
@@ -2855,9 +2798,6 @@
       <c r="AI19" s="6">
         <v>-17</v>
       </c>
-      <c r="AJ19" s="6">
-        <v>-17</v>
-      </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="2">
@@ -2965,9 +2905,6 @@
       <c r="AI20" s="6">
         <v>-18</v>
       </c>
-      <c r="AJ20" s="6">
-        <v>-18</v>
-      </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="7">
@@ -3075,9 +3012,6 @@
       <c r="AI21" s="6">
         <v>-19</v>
       </c>
-      <c r="AJ21" s="6">
-        <v>-19</v>
-      </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="2">
@@ -3185,9 +3119,6 @@
       <c r="AI22" s="6">
         <v>-20</v>
       </c>
-      <c r="AJ22" s="6">
-        <v>-20</v>
-      </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="2">
@@ -3295,9 +3226,6 @@
       <c r="AI23" s="6">
         <v>-21</v>
       </c>
-      <c r="AJ23" s="6">
-        <v>-21</v>
-      </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="2">
@@ -3405,9 +3333,6 @@
       <c r="AI24" s="6">
         <v>-22</v>
       </c>
-      <c r="AJ24" s="6">
-        <v>-22</v>
-      </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="2">
@@ -3515,9 +3440,6 @@
       <c r="AI25" s="6">
         <v>-23</v>
       </c>
-      <c r="AJ25" s="6">
-        <v>-23</v>
-      </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="7">
@@ -3625,9 +3547,6 @@
       <c r="AI26" s="6">
         <v>-24</v>
       </c>
-      <c r="AJ26" s="6">
-        <v>-24</v>
-      </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="2">
@@ -3735,9 +3654,6 @@
       <c r="AI27" s="4">
         <v>25</v>
       </c>
-      <c r="AJ27" s="4">
-        <v>25</v>
-      </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="2">
@@ -3845,9 +3761,6 @@
       <c r="AI28" s="4">
         <v>25</v>
       </c>
-      <c r="AJ28" s="4">
-        <v>25</v>
-      </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="2">
@@ -3955,9 +3868,6 @@
       <c r="AI29" s="6">
         <v>-25</v>
       </c>
-      <c r="AJ29" s="6">
-        <v>-25</v>
-      </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="2">
@@ -4065,9 +3975,6 @@
       <c r="AI30" s="6">
         <v>-26</v>
       </c>
-      <c r="AJ30" s="6">
-        <v>-26</v>
-      </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="7">
@@ -4175,9 +4082,6 @@
       <c r="AI31" s="6">
         <v>-27</v>
       </c>
-      <c r="AJ31" s="6">
-        <v>-27</v>
-      </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="2">
@@ -4285,9 +4189,6 @@
       <c r="AI32" s="6">
         <v>-28</v>
       </c>
-      <c r="AJ32" s="6">
-        <v>-28</v>
-      </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="2">
@@ -4395,9 +4296,6 @@
       <c r="AI33" s="6">
         <v>-29</v>
       </c>
-      <c r="AJ33" s="6">
-        <v>-29</v>
-      </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="2">
@@ -4505,9 +4403,6 @@
       <c r="AI34" s="6">
         <v>-30</v>
       </c>
-      <c r="AJ34" s="6">
-        <v>-30</v>
-      </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="2">
@@ -4615,9 +4510,6 @@
       <c r="AI35" s="6">
         <v>-31</v>
       </c>
-      <c r="AJ35" s="6">
-        <v>-31</v>
-      </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="7">
@@ -4725,9 +4617,6 @@
       <c r="AI36" s="6">
         <v>-32</v>
       </c>
-      <c r="AJ36" s="6">
-        <v>-32</v>
-      </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="2">
@@ -4835,9 +4724,6 @@
       <c r="AI37" s="6">
         <v>-33</v>
       </c>
-      <c r="AJ37" s="6">
-        <v>-33</v>
-      </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="2">
@@ -4945,9 +4831,6 @@
       <c r="AI38" s="6">
         <v>-34</v>
       </c>
-      <c r="AJ38" s="6">
-        <v>-34</v>
-      </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="2">
@@ -5055,9 +4938,6 @@
       <c r="AI39" s="6">
         <v>-35</v>
       </c>
-      <c r="AJ39" s="6">
-        <v>-35</v>
-      </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="2">
@@ -5165,9 +5045,6 @@
       <c r="AI40" s="6">
         <v>-36</v>
       </c>
-      <c r="AJ40" s="6">
-        <v>-36</v>
-      </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="7">
@@ -5275,9 +5152,6 @@
       <c r="AI41" s="6">
         <v>-37</v>
       </c>
-      <c r="AJ41" s="6">
-        <v>-37</v>
-      </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="2">
@@ -5385,9 +5259,6 @@
       <c r="AI42" s="6">
         <v>-38</v>
       </c>
-      <c r="AJ42" s="6">
-        <v>-38</v>
-      </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="2">
@@ -5495,9 +5366,6 @@
       <c r="AI43" s="6">
         <v>-39</v>
       </c>
-      <c r="AJ43" s="6">
-        <v>-39</v>
-      </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="2">
@@ -5605,9 +5473,6 @@
       <c r="AI44" s="6">
         <v>-40</v>
       </c>
-      <c r="AJ44" s="6">
-        <v>-40</v>
-      </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="2">
@@ -5715,9 +5580,6 @@
       <c r="AI45" s="6">
         <v>-41</v>
       </c>
-      <c r="AJ45" s="6">
-        <v>-41</v>
-      </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="7">
@@ -5825,9 +5687,6 @@
       <c r="AI46" s="6">
         <v>-42</v>
       </c>
-      <c r="AJ46" s="6">
-        <v>-42</v>
-      </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="2">
@@ -5935,9 +5794,6 @@
       <c r="AI47" s="6">
         <v>-43</v>
       </c>
-      <c r="AJ47" s="6">
-        <v>-43</v>
-      </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="2">
@@ -6045,9 +5901,6 @@
       <c r="AI48" s="6">
         <v>-44</v>
       </c>
-      <c r="AJ48" s="6">
-        <v>-44</v>
-      </c>
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="2">
@@ -6155,9 +6008,6 @@
       <c r="AI49" s="6">
         <v>-45</v>
       </c>
-      <c r="AJ49" s="6">
-        <v>-45</v>
-      </c>
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="2">
@@ -6265,9 +6115,6 @@
       <c r="AI50" s="6">
         <v>-46</v>
       </c>
-      <c r="AJ50" s="6">
-        <v>-46</v>
-      </c>
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="7">
@@ -6375,9 +6222,6 @@
       <c r="AI51" s="6">
         <v>-47</v>
       </c>
-      <c r="AJ51" s="6">
-        <v>-47</v>
-      </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="2">
@@ -6485,9 +6329,6 @@
       <c r="AI52" s="6">
         <v>-48</v>
       </c>
-      <c r="AJ52" s="6">
-        <v>-48</v>
-      </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="2">
@@ -6595,9 +6436,6 @@
       <c r="AI53" s="6">
         <v>-49</v>
       </c>
-      <c r="AJ53" s="6">
-        <v>-49</v>
-      </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" s="2">
@@ -6705,9 +6543,6 @@
       <c r="AI54" s="6">
         <v>-50</v>
       </c>
-      <c r="AJ54" s="6">
-        <v>-50</v>
-      </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="2">
@@ -6815,9 +6650,6 @@
       <c r="AI55" s="6">
         <v>-51</v>
       </c>
-      <c r="AJ55" s="6">
-        <v>-51</v>
-      </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="7">
@@ -6916,16 +6748,13 @@
       <c r="AF56" s="4">
         <v>54</v>
       </c>
-      <c r="AG56" s="4">
+      <c r="AG56" s="5">
+        <v>501</v>
+      </c>
+      <c r="AH56" s="4">
         <v>54</v>
       </c>
-      <c r="AH56" s="5">
-        <v>501</v>
-      </c>
-      <c r="AI56" s="4">
-        <v>54</v>
-      </c>
-      <c r="AJ56" s="5">
+      <c r="AI56" s="5">
         <v>501</v>
       </c>
     </row>
@@ -7035,9 +6864,6 @@
       <c r="AI57" s="6">
         <v>-52</v>
       </c>
-      <c r="AJ57" s="6">
-        <v>-52</v>
-      </c>
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="2">
@@ -7136,16 +6962,13 @@
       <c r="AF58" s="4">
         <v>56</v>
       </c>
-      <c r="AG58" s="4">
+      <c r="AG58" s="5">
+        <v>502</v>
+      </c>
+      <c r="AH58" s="4">
         <v>56</v>
       </c>
-      <c r="AH58" s="5">
-        <v>502</v>
-      </c>
-      <c r="AI58" s="4">
-        <v>56</v>
-      </c>
-      <c r="AJ58" s="5">
+      <c r="AI58" s="5">
         <v>502</v>
       </c>
     </row>
@@ -7255,9 +7078,6 @@
       <c r="AI59" s="6">
         <v>-53</v>
       </c>
-      <c r="AJ59" s="6">
-        <v>-53</v>
-      </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="2">
@@ -7365,9 +7185,6 @@
       <c r="AI60" s="6">
         <v>-54</v>
       </c>
-      <c r="AJ60" s="6">
-        <v>-54</v>
-      </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="7">
@@ -7475,9 +7292,6 @@
       <c r="AI61" s="5">
         <v>503</v>
       </c>
-      <c r="AJ61" s="5">
-        <v>503</v>
-      </c>
     </row>
     <row r="62" ht="15.75" customHeight="1">
       <c r="A62" s="2">
@@ -7585,9 +7399,6 @@
       <c r="AI62" s="6">
         <v>-55</v>
       </c>
-      <c r="AJ62" s="6">
-        <v>-55</v>
-      </c>
     </row>
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="2">
@@ -7695,9 +7506,6 @@
       <c r="AI63" s="5">
         <v>504</v>
       </c>
-      <c r="AJ63" s="5">
-        <v>504</v>
-      </c>
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="2">
@@ -7805,9 +7613,6 @@
       <c r="AI64" s="5">
         <v>503</v>
       </c>
-      <c r="AJ64" s="5">
-        <v>503</v>
-      </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="2">
@@ -7915,9 +7720,6 @@
       <c r="AI65" s="6">
         <v>-56</v>
       </c>
-      <c r="AJ65" s="6">
-        <v>-56</v>
-      </c>
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="7">
@@ -8007,14 +7809,14 @@
       <c r="AC66" s="9">
         <v>64</v>
       </c>
-      <c r="AD66" s="9">
+      <c r="AD66" s="8">
+        <v>-57</v>
+      </c>
+      <c r="AE66" s="9">
         <v>64</v>
       </c>
-      <c r="AE66" s="8">
+      <c r="AF66" s="8">
         <v>-57</v>
-      </c>
-      <c r="AF66" s="9">
-        <v>64</v>
       </c>
       <c r="AG66" s="8">
         <v>-57</v>
@@ -8023,9 +7825,6 @@
         <v>-57</v>
       </c>
       <c r="AI66" s="8">
-        <v>-57</v>
-      </c>
-      <c r="AJ66" s="8">
         <v>-57</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se arregló las direcciónes de los comentarios de una linea en la matríz
</commit_message>
<xml_diff>
--- a/src/main/resources/matrix.xlsx
+++ b/src/main/resources/matrix.xlsx
@@ -3338,107 +3338,107 @@
       <c r="A25" s="2">
         <v>23</v>
       </c>
-      <c r="B25" s="6">
-        <v>-23</v>
-      </c>
-      <c r="C25" s="6">
-        <v>-23</v>
-      </c>
-      <c r="D25" s="6">
-        <v>-23</v>
-      </c>
-      <c r="E25" s="6">
-        <v>-23</v>
-      </c>
-      <c r="F25" s="6">
-        <v>-23</v>
-      </c>
-      <c r="G25" s="6">
-        <v>-23</v>
-      </c>
-      <c r="H25" s="6">
-        <v>-23</v>
-      </c>
-      <c r="I25" s="6">
-        <v>-23</v>
-      </c>
-      <c r="J25" s="6">
-        <v>-23</v>
-      </c>
-      <c r="K25" s="6">
-        <v>-23</v>
-      </c>
-      <c r="L25" s="6">
-        <v>-23</v>
-      </c>
-      <c r="M25" s="6">
-        <v>-23</v>
-      </c>
-      <c r="N25" s="6">
-        <v>-23</v>
-      </c>
-      <c r="O25" s="6">
-        <v>-23</v>
-      </c>
-      <c r="P25" s="6">
-        <v>-23</v>
-      </c>
-      <c r="Q25" s="6">
-        <v>-23</v>
-      </c>
-      <c r="R25" s="6">
-        <v>-23</v>
-      </c>
-      <c r="S25" s="6">
-        <v>-23</v>
-      </c>
-      <c r="T25" s="6">
-        <v>-23</v>
-      </c>
-      <c r="U25" s="6">
-        <v>-23</v>
-      </c>
-      <c r="V25" s="6">
-        <v>-23</v>
-      </c>
-      <c r="W25" s="6">
-        <v>-23</v>
-      </c>
-      <c r="X25" s="6">
-        <v>-23</v>
-      </c>
-      <c r="Y25" s="6">
-        <v>-23</v>
-      </c>
-      <c r="Z25" s="6">
-        <v>-23</v>
-      </c>
-      <c r="AA25" s="6">
-        <v>-23</v>
-      </c>
-      <c r="AB25" s="6">
-        <v>-23</v>
-      </c>
-      <c r="AC25" s="6">
-        <v>-23</v>
-      </c>
-      <c r="AD25" s="6">
-        <v>-23</v>
-      </c>
-      <c r="AE25" s="6">
-        <v>-23</v>
-      </c>
-      <c r="AF25" s="6">
-        <v>-23</v>
+      <c r="B25" s="4">
+        <v>23</v>
+      </c>
+      <c r="C25" s="4">
+        <v>23</v>
+      </c>
+      <c r="D25" s="4">
+        <v>23</v>
+      </c>
+      <c r="E25" s="4">
+        <v>23</v>
+      </c>
+      <c r="F25" s="4">
+        <v>23</v>
+      </c>
+      <c r="G25" s="4">
+        <v>23</v>
+      </c>
+      <c r="H25" s="4">
+        <v>23</v>
+      </c>
+      <c r="I25" s="4">
+        <v>23</v>
+      </c>
+      <c r="J25" s="4">
+        <v>23</v>
+      </c>
+      <c r="K25" s="4">
+        <v>23</v>
+      </c>
+      <c r="L25" s="4">
+        <v>23</v>
+      </c>
+      <c r="M25" s="4">
+        <v>23</v>
+      </c>
+      <c r="N25" s="4">
+        <v>23</v>
+      </c>
+      <c r="O25" s="4">
+        <v>23</v>
+      </c>
+      <c r="P25" s="4">
+        <v>23</v>
+      </c>
+      <c r="Q25" s="4">
+        <v>23</v>
+      </c>
+      <c r="R25" s="4">
+        <v>23</v>
+      </c>
+      <c r="S25" s="4">
+        <v>23</v>
+      </c>
+      <c r="T25" s="4">
+        <v>23</v>
+      </c>
+      <c r="U25" s="4">
+        <v>23</v>
+      </c>
+      <c r="V25" s="4">
+        <v>23</v>
+      </c>
+      <c r="W25" s="4">
+        <v>23</v>
+      </c>
+      <c r="X25" s="4">
+        <v>23</v>
+      </c>
+      <c r="Y25" s="4">
+        <v>23</v>
+      </c>
+      <c r="Z25" s="4">
+        <v>23</v>
+      </c>
+      <c r="AA25" s="4">
+        <v>23</v>
+      </c>
+      <c r="AB25" s="4">
+        <v>23</v>
+      </c>
+      <c r="AC25" s="4">
+        <v>23</v>
+      </c>
+      <c r="AD25" s="4">
+        <v>23</v>
+      </c>
+      <c r="AE25" s="4">
+        <v>23</v>
+      </c>
+      <c r="AF25" s="4">
+        <v>23</v>
       </c>
       <c r="AG25" s="6">
         <v>-23</v>
       </c>
-      <c r="AH25" s="6">
-        <v>-23</v>
-      </c>
-      <c r="AI25" s="6">
-        <v>-23</v>
+      <c r="AH25" s="4">
+        <v>23</v>
+      </c>
+      <c r="AI25" s="4">
+        <v>23</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
Se arregló la dirección de los números en la matríz
</commit_message>
<xml_diff>
--- a/src/main/resources/matrix.xlsx
+++ b/src/main/resources/matrix.xlsx
@@ -7161,8 +7161,8 @@
       <c r="AA60" s="6">
         <v>-54</v>
       </c>
-      <c r="AB60" s="6">
-        <v>-54</v>
+      <c r="AB60" s="4">
+        <v>58</v>
       </c>
       <c r="AC60" s="6">
         <v>-54</v>

</xml_diff>

<commit_message>
Se modificó las etiquetas de las flechas en los estados de constantes de cadenas
</commit_message>
<xml_diff>
--- a/src/main/resources/matrix.xlsx
+++ b/src/main/resources/matrix.xlsx
@@ -6754,8 +6754,8 @@
       <c r="AH56" s="4">
         <v>54</v>
       </c>
-      <c r="AI56" s="5">
-        <v>501</v>
+      <c r="AI56" s="4">
+        <v>54</v>
       </c>
     </row>
     <row r="57" ht="15.75" customHeight="1">
@@ -6968,8 +6968,8 @@
       <c r="AH58" s="4">
         <v>56</v>
       </c>
-      <c r="AI58" s="5">
-        <v>502</v>
+      <c r="AI58" s="4">
+        <v>56</v>
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">

</xml_diff>